<commit_message>
Modificacion de formato PQRS
- agregada direccion y eliminacion de 2 filas despues de la cabecera
</commit_message>
<xml_diff>
--- a/formatos/reportePQRS_F-136.xlsx
+++ b/formatos/reportePQRS_F-136.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Código: GCSP-F-136</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t>SIGLAS</t>
-  </si>
-  <si>
-    <t>Avenida Calle 26 Nro. 59-51 Torre 4 y/o Calle 24A Nro. 59-42 Torre 4 Piso 2</t>
   </si>
   <si>
     <r>
@@ -355,19 +352,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">PBX: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>4848860-  www.ani.gov.co, Nit. 830125996-9</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -481,6 +465,15 @@
   <si>
     <t>PROYECTO CONCESIÓN VÍAS DEL NUS - VINUS</t>
   </si>
+  <si>
+    <t>Concesión Vías del NUS S.A.S. – VINUS</t>
+  </si>
+  <si>
+    <t>Calle 59 No. 48 – 35 Copacabana – Antioquia (Kilometro 4 + 500 Autopista Norte)</t>
+  </si>
+  <si>
+    <t>PBX: (574) 401 2277 FAX: (574) 401 2277</t>
+  </si>
 </sst>
 </file>
 
@@ -558,8 +551,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Arial"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -807,10 +802,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -866,35 +862,67 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -927,42 +955,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1355,10 +1358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB984"/>
+  <dimension ref="A1:AB982"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C9"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A12" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:Z22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1390,98 +1393,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="48" t="s">
-        <v>48</v>
+      <c r="A1" s="48"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="58" t="s">
+        <v>46</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="54" t="s">
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="56"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="38"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="42" t="s">
+      <c r="A2" s="42"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="57" t="s">
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="42"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
-      <c r="Z2" s="56"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="38"/>
     </row>
     <row r="3" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="41"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
-      <c r="T3" s="47"/>
-      <c r="U3" s="41"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="57" t="s">
+      <c r="A3" s="44"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="56"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="44"/>
+      <c r="V3" s="45"/>
+      <c r="W3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="X3" s="55"/>
-      <c r="Y3" s="55"/>
-      <c r="Z3" s="56"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="38"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
@@ -1511,294 +1514,303 @@
       <c r="Y4" s="5"/>
       <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="6"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="6"/>
-    </row>
-    <row r="7" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+    <row r="5" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="25" t="s">
+      <c r="B5" s="30"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E5" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="25" t="s">
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="25" t="s">
+      <c r="K5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="25" t="s">
+      <c r="L5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="25" t="s">
+      <c r="M5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="28" t="s">
+      <c r="N5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="34"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="28" t="s">
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="T7" s="29"/>
-      <c r="U7" s="25" t="s">
+      <c r="T5" s="26"/>
+      <c r="U5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="V7" s="25" t="s">
+      <c r="V5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="W7" s="28" t="s">
+      <c r="W5" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="X7" s="29"/>
-      <c r="Y7" s="25" t="s">
+      <c r="X5" s="26"/>
+      <c r="Y5" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="Z7" s="59" t="s">
+      <c r="Z5" s="46" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+    <row r="6" spans="1:28" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="7" t="s">
+      <c r="D6" s="24"/>
+      <c r="E6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="64"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="7" t="s">
+      <c r="J6" s="35"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="O6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="P6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="Q8" s="7" t="s">
+      <c r="Q6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="7" t="s">
+      <c r="R6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="S8" s="7" t="s">
+      <c r="S6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="T8" s="7" t="s">
+      <c r="T6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="U8" s="27"/>
-      <c r="V8" s="26"/>
-      <c r="W8" s="7" t="s">
+      <c r="U6" s="34"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="X8" s="7" t="s">
+      <c r="X6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="60"/>
-    </row>
-    <row r="9" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="65"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="9"/>
-      <c r="X9" s="9"/>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="12"/>
-    </row>
-    <row r="10" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="14"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="W11" s="17"/>
-      <c r="X11" s="17"/>
-    </row>
-    <row r="12" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="47"/>
+    </row>
+    <row r="7" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="12"/>
+    </row>
+    <row r="8" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+    </row>
+    <row r="10" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="30" t="s">
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="22"/>
-      <c r="U12" s="22"/>
-      <c r="V12" s="22"/>
-      <c r="W12" s="22"/>
-      <c r="X12" s="22"/>
-      <c r="Y12" s="22"/>
-      <c r="Z12" s="23"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="32"/>
+      <c r="X10" s="32"/>
+      <c r="Y10" s="32"/>
+      <c r="Z10" s="33"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A11" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="50"/>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="50"/>
+      <c r="S11" s="50"/>
+      <c r="T11" s="50"/>
+      <c r="U11" s="50"/>
+      <c r="V11" s="50"/>
+      <c r="W11" s="50"/>
+      <c r="X11" s="50"/>
+      <c r="Y11" s="50"/>
+      <c r="Z11" s="45"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A12" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="32"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="33"/>
+      <c r="AB12" s="20"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
-        <v>35</v>
+      <c r="A13" s="64" t="s">
+        <v>37</v>
       </c>
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
@@ -1812,8 +1824,8 @@
       <c r="K13" s="32"/>
       <c r="L13" s="32"/>
       <c r="M13" s="33"/>
-      <c r="N13" s="31" t="s">
-        <v>35</v>
+      <c r="N13" s="64" t="s">
+        <v>38</v>
       </c>
       <c r="O13" s="32"/>
       <c r="P13" s="32"/>
@@ -1829,73 +1841,61 @@
       <c r="Z13" s="33"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
-        <v>36</v>
+      <c r="A14" s="64" t="s">
+        <v>39</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="22"/>
-      <c r="T14" s="22"/>
-      <c r="U14" s="22"/>
-      <c r="V14" s="22"/>
-      <c r="W14" s="22"/>
-      <c r="X14" s="22"/>
-      <c r="Y14" s="22"/>
-      <c r="Z14" s="23"/>
-      <c r="AB14" s="20"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="32"/>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="32"/>
+      <c r="Z14" s="33"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
-      <c r="U15" s="22"/>
-      <c r="V15" s="22"/>
-      <c r="W15" s="22"/>
-      <c r="X15" s="22"/>
-      <c r="Y15" s="22"/>
-      <c r="Z15" s="23"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
-        <v>39</v>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+    </row>
+    <row r="16" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>40</v>
       </c>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
@@ -1908,33 +1908,34 @@
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
       <c r="L16" s="22"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="22"/>
-      <c r="U16" s="22"/>
-      <c r="V16" s="22"/>
-      <c r="W16" s="22"/>
-      <c r="X16" s="22"/>
-      <c r="Y16" s="22"/>
-      <c r="Z16" s="23"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+    </row>
+    <row r="17" spans="1:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
       <c r="N17" s="17"/>
       <c r="O17" s="17"/>
       <c r="P17" s="17"/>
@@ -1947,204 +1948,214 @@
       <c r="X17" s="17"/>
     </row>
     <row r="18" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-      <c r="T18" s="17"/>
-      <c r="U18" s="17"/>
-      <c r="W18" s="17"/>
-      <c r="X18" s="17"/>
-    </row>
-    <row r="19" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
+      <c r="A18" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
-      <c r="U19" s="17"/>
-      <c r="W19" s="17"/>
-      <c r="X19" s="17"/>
-    </row>
-    <row r="20" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="22"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22"/>
+      <c r="Z18" s="22"/>
+    </row>
+    <row r="19" spans="1:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="61" t="s">
-        <v>41</v>
-      </c>
-      <c r="O20" s="39"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="39"/>
-      <c r="R20" s="39"/>
-      <c r="S20" s="39"/>
-      <c r="T20" s="39"/>
-      <c r="U20" s="39"/>
-      <c r="V20" s="39"/>
-      <c r="W20" s="39"/>
-      <c r="X20" s="39"/>
-      <c r="Y20" s="39"/>
-      <c r="Z20" s="39"/>
-    </row>
-    <row r="21" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22"/>
+      <c r="U19" s="22"/>
+      <c r="V19" s="22"/>
+      <c r="W19" s="22"/>
+      <c r="X19" s="22"/>
+      <c r="Y19" s="22"/>
+      <c r="Z19" s="22"/>
+    </row>
+    <row r="20" spans="1:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="62" t="s">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="17"/>
+    </row>
+    <row r="21" spans="1:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="O21" s="39"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="39"/>
-      <c r="S21" s="39"/>
-      <c r="T21" s="39"/>
-      <c r="U21" s="39"/>
-      <c r="V21" s="39"/>
-      <c r="W21" s="39"/>
-      <c r="X21" s="39"/>
-      <c r="Y21" s="39"/>
-      <c r="Z21" s="39"/>
-    </row>
-    <row r="22" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
-      <c r="U22" s="17"/>
-      <c r="W22" s="17"/>
-      <c r="X22" s="17"/>
-    </row>
-    <row r="23" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="17"/>
+      <c r="W21" s="17"/>
+      <c r="X21" s="17"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A22" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
-      <c r="U23" s="17"/>
-      <c r="W23" s="17"/>
-      <c r="X23" s="17"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="66"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="66"/>
+      <c r="M22" s="66"/>
+      <c r="N22" s="66"/>
+      <c r="O22" s="66"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="66"/>
+      <c r="R22" s="66"/>
+      <c r="S22" s="66"/>
+      <c r="T22" s="66"/>
+      <c r="U22" s="66"/>
+      <c r="V22" s="66"/>
+      <c r="W22" s="66"/>
+      <c r="X22" s="66"/>
+      <c r="Y22" s="66"/>
+      <c r="Z22" s="66"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A23" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="66"/>
+      <c r="K23" s="66"/>
+      <c r="L23" s="66"/>
+      <c r="M23" s="66"/>
+      <c r="N23" s="66"/>
+      <c r="O23" s="66"/>
+      <c r="P23" s="66"/>
+      <c r="Q23" s="66"/>
+      <c r="R23" s="66"/>
+      <c r="S23" s="66"/>
+      <c r="T23" s="66"/>
+      <c r="U23" s="66"/>
+      <c r="V23" s="66"/>
+      <c r="W23" s="66"/>
+      <c r="X23" s="66"/>
+      <c r="Y23" s="66"/>
+      <c r="Z23" s="66"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17"/>
-      <c r="T24" s="17"/>
-      <c r="U24" s="17"/>
-      <c r="W24" s="17"/>
-      <c r="X24" s="17"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
+      <c r="A24" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="66"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="66"/>
+      <c r="J24" s="66"/>
+      <c r="K24" s="66"/>
+      <c r="L24" s="66"/>
+      <c r="M24" s="66"/>
+      <c r="N24" s="66"/>
+      <c r="O24" s="66"/>
+      <c r="P24" s="66"/>
+      <c r="Q24" s="66"/>
+      <c r="R24" s="66"/>
+      <c r="S24" s="66"/>
+      <c r="T24" s="66"/>
+      <c r="U24" s="66"/>
+      <c r="V24" s="66"/>
+      <c r="W24" s="66"/>
+      <c r="X24" s="66"/>
+      <c r="Y24" s="66"/>
+      <c r="Z24" s="66"/>
+    </row>
+    <row r="25" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="67"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
@@ -24175,93 +24186,51 @@
       <c r="W982" s="17"/>
       <c r="X982" s="17"/>
     </row>
-    <row r="983" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A983" s="17"/>
-      <c r="B983" s="17"/>
-      <c r="C983" s="17"/>
-      <c r="E983" s="17"/>
-      <c r="F983" s="17"/>
-      <c r="G983" s="17"/>
-      <c r="H983" s="17"/>
-      <c r="I983" s="17"/>
-      <c r="K983" s="17"/>
-      <c r="L983" s="17"/>
-      <c r="M983" s="17"/>
-      <c r="N983" s="17"/>
-      <c r="O983" s="17"/>
-      <c r="P983" s="17"/>
-      <c r="Q983" s="17"/>
-      <c r="R983" s="17"/>
-      <c r="S983" s="17"/>
-      <c r="T983" s="17"/>
-      <c r="U983" s="17"/>
-      <c r="W983" s="17"/>
-      <c r="X983" s="17"/>
-    </row>
-    <row r="984" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A984" s="17"/>
-      <c r="B984" s="17"/>
-      <c r="C984" s="17"/>
-      <c r="E984" s="17"/>
-      <c r="F984" s="17"/>
-      <c r="G984" s="17"/>
-      <c r="H984" s="17"/>
-      <c r="I984" s="17"/>
-      <c r="K984" s="17"/>
-      <c r="L984" s="17"/>
-      <c r="M984" s="17"/>
-      <c r="N984" s="17"/>
-      <c r="O984" s="17"/>
-      <c r="P984" s="17"/>
-      <c r="Q984" s="17"/>
-      <c r="R984" s="17"/>
-      <c r="S984" s="17"/>
-      <c r="T984" s="17"/>
-      <c r="U984" s="17"/>
-      <c r="W984" s="17"/>
-      <c r="X984" s="17"/>
-    </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="A20:M20"/>
-    <mergeCell ref="A22:M22"/>
-    <mergeCell ref="A21:M21"/>
-    <mergeCell ref="A23:M23"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="N20:Z20"/>
-    <mergeCell ref="N21:Z21"/>
-    <mergeCell ref="A18:M18"/>
-    <mergeCell ref="A19:M19"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A7:C7"/>
+  <mergeCells count="43">
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A22:Z22"/>
+    <mergeCell ref="A23:Z23"/>
+    <mergeCell ref="A24:Z24"/>
     <mergeCell ref="A12:M12"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="N14:Z14"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="N10:Z10"/>
+    <mergeCell ref="N11:Z11"/>
+    <mergeCell ref="N12:Z12"/>
+    <mergeCell ref="N13:Z13"/>
+    <mergeCell ref="A13:M13"/>
+    <mergeCell ref="A14:M14"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="A11:M11"/>
+    <mergeCell ref="E2:T3"/>
+    <mergeCell ref="E1:T1"/>
+    <mergeCell ref="E5:I5"/>
     <mergeCell ref="W1:Z1"/>
     <mergeCell ref="W2:Z2"/>
     <mergeCell ref="W3:Z3"/>
     <mergeCell ref="U1:V3"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="A13:M13"/>
-    <mergeCell ref="E2:T3"/>
-    <mergeCell ref="E1:T1"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="A14:M14"/>
-    <mergeCell ref="N16:Z16"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="N12:Z12"/>
-    <mergeCell ref="N13:Z13"/>
-    <mergeCell ref="N14:Z14"/>
-    <mergeCell ref="N15:Z15"/>
-    <mergeCell ref="A15:M15"/>
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="A18:M18"/>
+    <mergeCell ref="A20:M20"/>
+    <mergeCell ref="A19:M19"/>
+    <mergeCell ref="A21:M21"/>
+    <mergeCell ref="Y5:Y6"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="N18:Z18"/>
+    <mergeCell ref="N19:Z19"/>
     <mergeCell ref="A16:M16"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="A17:M17"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>